<commit_message>
Toma de datos (máquina 2)
</commit_message>
<xml_diff>
--- a/Docs/Gráficas máquina 2.xlsx
+++ b/Docs/Gráficas máquina 2.xlsx
@@ -5,29 +5,38 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Reto 4\Reto4-G10\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Namek\Desktop\Clase de Estructuras de Datos y Algoritmos\Segundo trimestre\Reto 4\Reto4-G10\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04041665-31A7-4220-9BA0-863EF52EFCB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4641E5AD-B9DD-4954-9EB3-C6CF653B9FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{674F7855-6ABB-4172-9BD7-8DDF58622BAF}"/>
+    <workbookView xWindow="17190" yWindow="3915" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{674F7855-6ABB-4172-9BD7-8DDF58622BAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos de rendimiento" sheetId="1" r:id="rId1"/>
     <sheet name="Gráfico1" sheetId="4" r:id="rId2"/>
     <sheet name="Gráfico2" sheetId="6" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>Requerimiento</t>
   </si>
@@ -54,6 +63,21 @@
   </si>
   <si>
     <t>Carga de datos</t>
+  </si>
+  <si>
+    <t>From: Redondo Beach, CA, United States</t>
+  </si>
+  <si>
+    <t>To: Vung Tau, Vietnam</t>
+  </si>
+  <si>
+    <t>From: Colombia</t>
+  </si>
+  <si>
+    <t>To: Indonesia</t>
+  </si>
+  <si>
+    <t>Sunny Isles, FL, United States</t>
   </si>
 </sst>
 </file>
@@ -155,41 +179,65 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -286,8 +334,9 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -304,17 +353,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -345,7 +392,6 @@
                 <a:endParaRPr lang="es-CO"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="t"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -405,10 +451,27 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>865.47180000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3682.3780000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>69.504599999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1114.0134</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1390.2539999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5358000000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-AB9C-4144-9B02-3FDE99586C66}"/>
@@ -416,7 +479,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -424,11 +486,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
+        <c:gapWidth val="150"/>
         <c:axId val="355150376"/>
         <c:axId val="355153000"/>
-        <c:extLst/>
-      </c:lineChart>
+      </c:barChart>
       <c:catAx>
         <c:axId val="355150376"/>
         <c:scaling>
@@ -854,8 +915,9 @@
           <c:h val="0.76414449115816818"/>
         </c:manualLayout>
       </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
@@ -872,17 +934,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -913,7 +973,6 @@
                 <a:endParaRPr lang="es-CO"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="t"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -973,10 +1032,27 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4626.8756000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>121.2606</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="#,##0.000">
+                  <c:v>587.53899999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.087399999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.6922</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.918800000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-BF96-4BA8-A925-9AF4D054CAE7}"/>
@@ -984,7 +1060,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -992,10 +1067,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
         <c:axId val="92092336"/>
         <c:axId val="92093976"/>
-      </c:lineChart>
+      </c:barChart>
       <c:catAx>
         <c:axId val="92092336"/>
         <c:scaling>
@@ -2366,7 +2442,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{C2BD6488-78FB-4B14-AE4F-1C07C56BD97A}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="95" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2377,7 +2453,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3E82B2E1-4E81-4ADC-AE54-9649EDC9AEE4}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2388,7 +2464,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8665535" cy="6282070"/>
+    <xdr:ext cx="9304587" cy="6077107"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -2421,7 +2497,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8665535" cy="6282070"/>
+    <xdr:ext cx="9294395" cy="6075947"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -2747,158 +2823,220 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2B8949-CC7B-4468-84E4-E8B7F9651F12}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" customWidth="1"/>
-    <col min="2" max="2" width="34.6640625" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="B1" s="12"/>
-      <c r="C1" s="3"/>
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="4"/>
+      <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="16" t="s">
+    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="15">
+    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="17"/>
+      <c r="C3" s="8">
+        <v>865.47180000000003</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="15">
+    <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="9">
+        <v>3682.3780000000002</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="15">
+    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="9">
+        <v>69.504599999999996</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="15">
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="11">
+        <v>1114.0134</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="15">
+    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="11">
+        <v>1390.2539999999999</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="15">
+    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="8"/>
+      <c r="C8" s="11">
+        <v>2.5358000000000001</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="12"/>
     </row>
-    <row r="9" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="10"/>
+    <row r="9" spans="1:5" s="13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="14"/>
+      <c r="E9" s="15"/>
     </row>
-    <row r="10" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="10"/>
+    <row r="10" spans="1:5" s="13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="14"/>
+      <c r="E10" s="15"/>
     </row>
-    <row r="11" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="10"/>
+    <row r="11" spans="1:5" s="13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="14"/>
+      <c r="E11" s="15"/>
     </row>
-    <row r="12" spans="1:3" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="C12" s="11"/>
+    <row r="12" spans="1:5" s="13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="16"/>
+      <c r="E12" s="15"/>
     </row>
-    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="B13" s="16" t="s">
+    <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="15">
+    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>0</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1">
+        <v>4626.8756000000003</v>
+      </c>
     </row>
-    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="15">
+    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>1</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1">
+        <v>121.2606</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="15">
+    <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>2</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="18">
+        <v>587.53899999999999</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="15">
+    <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>3</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1">
+        <v>27.087399999999999</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="15">
+    <row r="18" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>4</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="1">
+        <v>19.6922</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="15">
+    <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>5</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1"/>
+      <c r="C19" s="1">
+        <v>22.918800000000001</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>